<commit_message>
alle gruppen in der übersicht
</commit_message>
<xml_diff>
--- a/data/Gruppen Schulreise 2016.xlsx
+++ b/data/Gruppen Schulreise 2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">sort_order</t>
   </si>
@@ -64,10 +64,10 @@
     <t xml:space="preserve">Jan</t>
   </si>
   <si>
-    <t xml:space="preserve">079 105 59 63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079 157 01 03</t>
+    <t xml:space="preserve">079 105 59 63 (Jan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 157 01 03 (Simon)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 2</t>
@@ -82,10 +82,16 @@
     <t xml:space="preserve">Silvan</t>
   </si>
   <si>
-    <t xml:space="preserve">079 127 10 20 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">077 457 67 73</t>
+    <t xml:space="preserve">Noah (mi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 127 10 20 (Silvan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">077 457 67 73 (Silas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">078 925 94 26 (Noah, mi)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 3</t>
@@ -100,10 +106,16 @@
     <t xml:space="preserve">Diego</t>
   </si>
   <si>
-    <t xml:space="preserve">079 665 41 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079 932 97 02</t>
+    <t xml:space="preserve">Fabio (mi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 665 41 25 (Diego)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 932 97 02 (Michael)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 108 67 31 (Fabio, mi)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 4</t>
@@ -118,10 +130,10 @@
     <t xml:space="preserve">Nico</t>
   </si>
   <si>
-    <t xml:space="preserve">078 925 94 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079 108 67 31</t>
+    <t xml:space="preserve">078 925 94 26 (Noah)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 108 67 31 (Fabio)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 5</t>
@@ -136,10 +148,10 @@
     <t xml:space="preserve">Lukas</t>
   </si>
   <si>
-    <t xml:space="preserve">076 501 49 69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">077 991 24 91</t>
+    <t xml:space="preserve">076 501 49 69 (Dario)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">077 991 24 91 (Mojtaba)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 6</t>
@@ -154,79 +166,94 @@
     <t xml:space="preserve">Yannick</t>
   </si>
   <si>
-    <t xml:space="preserve">079 855 58 05 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">077 486 36 85</t>
+    <t xml:space="preserve">079 855 58 05 (Yannick)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">077 486 36 85 (Yelin)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 7</t>
   </si>
   <si>
+    <t xml:space="preserve">Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joshua</t>
   </si>
   <si>
+    <t xml:space="preserve">078 647 17 95 (Joshua)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">078 709 88 33 (Mike)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 495 37 19 (Luc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gruppe 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jasmin (Do)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 723 30 08 (Flavia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 789 81 76 (Fabiana)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gruppe 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 732 76 06 (Adina)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 957 07 02 (Lara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gruppe 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nadine</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fanny</t>
   </si>
   <si>
-    <t xml:space="preserve">Luc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">078 647 17 95 (joshua)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079 546 19 60 (fanny)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">076 495 37 19 (luc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gruppe 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flavia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olivia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jasmin (Do)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">076 723 30 08 (flavia)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079 789 81 76 (fabiana)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gruppe 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gruppe 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nadine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike</t>
+    <t xml:space="preserve">079 397 47 56 (Moana)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 248 11 97 (Nadine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 546 19 60 (Fanny)</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppe 11</t>
@@ -241,6 +268,12 @@
     <t xml:space="preserve">Danielle</t>
   </si>
   <si>
+    <t xml:space="preserve">079 191 55 91 (Michelle)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 283 34 38 (Danielle)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gruppe 12</t>
   </si>
   <si>
@@ -253,6 +286,12 @@
     <t xml:space="preserve">Emilie</t>
   </si>
   <si>
+    <t xml:space="preserve">079 127 36 81 (Emilie)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 305 90 99 (Nathalie)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gruppe 13</t>
   </si>
   <si>
@@ -268,6 +307,12 @@
     <t xml:space="preserve">Suena</t>
   </si>
   <si>
+    <t xml:space="preserve">079 732 64 48 (Suena)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079 474 40 43 (Chiara S.)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gruppe 14</t>
   </si>
   <si>
@@ -278,6 +323,9 @@
   </si>
   <si>
     <t xml:space="preserve">Timon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 349 44 05 (Valentin)</t>
   </si>
 </sst>
 </file>
@@ -366,7 +414,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,6 +424,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,16 +455,16 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,21 +506,23 @@
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -473,20 +531,26 @@
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,22 +558,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,94 +587,101 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,120 +689,158 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>81</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,17 +848,23 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>